<commit_message>
Update Burn Up Chart and Scrum Board
</commit_message>
<xml_diff>
--- a/info/Burn Up Chart - Sprint 3.xlsx
+++ b/info/Burn Up Chart - Sprint 3.xlsx
@@ -208,6 +208,9 @@
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -289,11 +292,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="252356072"/>
-        <c:axId val="252355680"/>
+        <c:axId val="312470664"/>
+        <c:axId val="312459688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="252356072"/>
+        <c:axId val="312470664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -350,12 +353,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252355680"/>
+        <c:crossAx val="312459688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="252355680"/>
+        <c:axId val="312459688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -472,7 +475,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252356072"/>
+        <c:crossAx val="312470664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1410,7 +1413,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,6 +1443,9 @@
       </c>
       <c r="C2">
         <v>1</v>
+      </c>
+      <c r="D2">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Scrum Board and Burn Up Chart
</commit_message>
<xml_diff>
--- a/info/Burn Up Chart - Sprint 3.xlsx
+++ b/info/Burn Up Chart - Sprint 3.xlsx
@@ -211,6 +211,12 @@
                 <c:pt idx="1">
                   <c:v>13</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -292,11 +298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="312470664"/>
-        <c:axId val="312459688"/>
+        <c:axId val="257353448"/>
+        <c:axId val="257354232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="312470664"/>
+        <c:axId val="257353448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -353,12 +359,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312459688"/>
+        <c:crossAx val="257354232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="312459688"/>
+        <c:axId val="257354232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -475,7 +481,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312470664"/>
+        <c:crossAx val="257353448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1413,7 +1419,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,6 +1461,9 @@
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4">
@@ -1462,6 +1471,9 @@
       </c>
       <c r="C4">
         <v>3</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>